<commit_message>
update0530 logs 1.auto data loading from wind 2.a log for predictions 3.clear all
</commit_message>
<xml_diff>
--- a/预测结果.xlsx
+++ b/预测结果.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9420" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="55">
   <si>
     <t>日期</t>
   </si>
@@ -188,10 +188,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
@@ -220,14 +220,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,38 +241,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,10 +271,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -327,13 +320,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -341,6 +327,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -362,6 +355,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -390,6 +390,48 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -402,7 +444,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,85 +546,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -504,73 +558,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -648,21 +648,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -674,6 +659,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -696,16 +696,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -738,151 +738,196 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
@@ -900,59 +945,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1303,261 +1306,312 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B7"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="4" width="10.7777777777778" customWidth="1"/>
-    <col min="5" max="5" width="16.4444444444444" style="14" customWidth="1"/>
+    <col min="5" max="5" width="16.4444444444444" style="1" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="13" style="15" customWidth="1"/>
+    <col min="7" max="7" width="13" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.4444444444444" customWidth="1"/>
     <col min="9" max="9" width="12.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="19" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="16">
+      <c r="A3" s="3">
         <v>5.21</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="9">
         <v>2.7825</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="22">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="26">
         <v>2.9218</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="13">
-        <f>ABS(E3-B3)</f>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H8" si="0">ABS(E3-B3)</f>
         <v>0.1393</v>
       </c>
-      <c r="I3" s="24">
-        <f>H3/B3</f>
+      <c r="I3" s="13">
+        <f t="shared" ref="I3:I8" si="1">H3/B3</f>
         <v>0.050062893081761</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="16">
+      <c r="A4" s="3">
         <v>5.22</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="9">
         <v>2.775</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <f>B4-B3</f>
         <v>-0.00750000000000028</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="13">
         <f>C4/B3</f>
         <v>-0.00269541778975751</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="26">
         <v>2.9206</v>
       </c>
-      <c r="F4" s="13">
-        <f>E4-E3</f>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F9" si="2">E4-E3</f>
         <v>-0.00120000000000031</v>
       </c>
-      <c r="G4" s="25">
-        <f>F4/E3</f>
+      <c r="G4" s="14">
+        <f t="shared" ref="G4:G9" si="3">F4/E3</f>
         <v>-0.000410705729345031</v>
       </c>
-      <c r="H4" s="13">
-        <f>ABS(E4-B4)</f>
+      <c r="H4" s="10">
+        <f t="shared" si="0"/>
         <v>0.1456</v>
       </c>
-      <c r="I4" s="24">
-        <f>H4/B4</f>
+      <c r="I4" s="13">
+        <f t="shared" si="1"/>
         <v>0.0524684684684685</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="16">
+      <c r="A5" s="3">
         <v>5.23</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="9">
         <v>2.7675</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="10">
         <f>B5-B4</f>
         <v>-0.00749999999999984</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="13">
         <f>C5/B4</f>
         <v>-0.00270270270270265</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="26">
         <v>2.9195</v>
       </c>
-      <c r="F5" s="13">
-        <f>E5-E4</f>
+      <c r="F5" s="10">
+        <f t="shared" si="2"/>
         <v>-0.00109999999999966</v>
       </c>
-      <c r="G5" s="25">
-        <f>F5/E4</f>
+      <c r="G5" s="14">
+        <f t="shared" si="3"/>
         <v>-0.000376634938026315</v>
       </c>
-      <c r="H5" s="13">
-        <f>ABS(E5-B5)</f>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
         <v>0.152</v>
       </c>
-      <c r="I5" s="24">
-        <f>H5/B5</f>
+      <c r="I5" s="13">
+        <f t="shared" si="1"/>
         <v>0.0549232158988257</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="16">
+      <c r="A6" s="3">
         <v>5.24</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="9">
         <v>2.765</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="10">
         <f>B6-B5</f>
         <v>-0.00249999999999995</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="13">
         <f>C6/B5</f>
         <v>-0.000903342366756983</v>
       </c>
-      <c r="E6" s="22">
+      <c r="E6" s="26">
         <v>2.9186</v>
       </c>
-      <c r="F6" s="13">
-        <f>E6-E5</f>
+      <c r="F6" s="10">
+        <f t="shared" si="2"/>
         <v>-0.000900000000000123</v>
       </c>
-      <c r="G6" s="25">
-        <f>F6/E5</f>
+      <c r="G6" s="14">
+        <f t="shared" si="3"/>
         <v>-0.000308271964377504</v>
       </c>
-      <c r="H6" s="13">
-        <f>ABS(E6-B6)</f>
+      <c r="H6" s="10">
+        <f t="shared" si="0"/>
         <v>0.1536</v>
       </c>
-      <c r="I6" s="24">
-        <f>H6/B6</f>
+      <c r="I6" s="13">
+        <f t="shared" si="1"/>
         <v>0.0555515370705244</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="16">
+      <c r="A7" s="3">
         <v>5.25</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="9">
         <v>2.7575</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="10">
         <f>B7-B6</f>
         <v>-0.00750000000000028</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="13">
         <f>C7/B6</f>
         <v>-0.0027124773960218</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="26">
         <v>2.9193</v>
       </c>
-      <c r="F7" s="13">
-        <f>E7-E6</f>
+      <c r="F7" s="10">
+        <f t="shared" si="2"/>
         <v>0.000699999999999701</v>
       </c>
-      <c r="G7" s="25">
-        <f>F7/E6</f>
+      <c r="G7" s="14">
+        <f t="shared" si="3"/>
         <v>0.000239841019666861</v>
       </c>
-      <c r="H7" s="13">
-        <f>ABS(E7-B7)</f>
+      <c r="H7" s="10">
+        <f t="shared" si="0"/>
         <v>0.1618</v>
       </c>
-      <c r="I7" s="24">
-        <f>H7/B7</f>
+      <c r="I7" s="13">
+        <f t="shared" si="1"/>
         <v>0.0586763372620127</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="22">
+      <c r="A8" s="3">
+        <v>5.26</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2.71</v>
+      </c>
+      <c r="C8" s="10">
+        <f>B8-B7</f>
+        <v>-0.0474999999999999</v>
+      </c>
+      <c r="D8" s="13">
+        <f>C8/B7</f>
+        <v>-0.0172257479601088</v>
+      </c>
+      <c r="E8" s="26">
         <v>2.9165</v>
       </c>
-      <c r="F8" s="13">
-        <f>E8-E7</f>
+      <c r="F8" s="10">
+        <f t="shared" si="2"/>
         <v>-0.00279999999999969</v>
       </c>
-      <c r="G8" s="25">
-        <f>F8/E7</f>
+      <c r="G8" s="14">
+        <f t="shared" si="3"/>
         <v>-0.000959134038981842</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="H8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.2065</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="1"/>
+        <v>0.0761992619926199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3">
+        <v>5.27</v>
+      </c>
+      <c r="B9" s="15">
+        <v>2.6974</v>
+      </c>
+      <c r="C9" s="10">
+        <f>B9-B8</f>
+        <v>-0.0125999999999999</v>
+      </c>
+      <c r="D9" s="13">
+        <f>C9/B8</f>
+        <v>-0.00464944649446492</v>
+      </c>
+      <c r="E9" s="26">
+        <v>2.8973</v>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.0192000000000001</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="3"/>
+        <v>-0.00658323332761876</v>
+      </c>
+      <c r="H9" s="10">
+        <f>ABS(E9-B9)</f>
+        <v>0.1999</v>
+      </c>
+      <c r="I9" s="13">
+        <f>H9/B9</f>
+        <v>0.0741084006821383</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1569,10 +1623,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:O32"/>
+  <dimension ref="A2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1585,10 +1639,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:15">
-      <c r="D2" s="1">
+      <c r="D2" s="16">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="16">
         <v>2</v>
       </c>
       <c r="F2">
@@ -1609,7 +1663,7 @@
       <c r="K2">
         <v>8</v>
       </c>
-      <c r="L2" s="1">
+      <c r="L2" s="16">
         <v>9</v>
       </c>
       <c r="M2" t="s">
@@ -1623,617 +1677,672 @@
       </c>
     </row>
     <row r="3" spans="2:15">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="18">
         <v>3.24160766601562</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="18">
         <v>3.2353458404541</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="19">
         <v>2.72789239883422</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="19">
         <v>2.60072445869445</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="19">
         <v>2.83023905754089</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="19">
         <v>2.96590185165405</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="19">
         <v>2.67520380020141</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="19">
         <v>2.79683423042297</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="18">
         <v>3.22209668159484</v>
       </c>
       <c r="M3">
-        <f>AVERAGE(D3:L3)</f>
+        <f t="shared" ref="M3:M9" si="0">AVERAGE(D3:L3)</f>
         <v>2.92176066504584</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="10">
         <v>2.7825</v>
       </c>
       <c r="O3">
-        <f>AVERAGE(F3,G3,H3,I3,J3,K3)</f>
+        <f t="shared" ref="O3:O9" si="1">AVERAGE(F3,G3,H3,I3,J3,K3)</f>
         <v>2.76613263289133</v>
       </c>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="18">
         <v>3.24160766601562</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="18">
         <v>3.2353458404541</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="19">
         <v>2.72151660919189</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="19">
         <v>2.59670352935791</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="19">
         <v>2.8299651145935</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="19">
         <v>2.97193145751953</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="19">
         <v>2.67442893981933</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="19">
         <v>2.79186296463012</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="18">
         <v>3.22209668159484</v>
       </c>
       <c r="M4">
-        <f>AVERAGE(D4:L4)</f>
+        <f t="shared" si="0"/>
         <v>2.92060653368632</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="10">
         <v>2.775</v>
       </c>
       <c r="O4">
-        <f>AVERAGE(F4,G4,H4,I4,J4,K4)</f>
+        <f t="shared" si="1"/>
         <v>2.76440143585205</v>
       </c>
     </row>
     <row r="5" spans="2:15">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="18">
         <v>3.24160766601562</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="18">
         <v>3.2353458404541</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="19">
         <v>2.71561288833618</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="19">
         <v>2.59289264678955</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="19">
         <v>2.82972121238708</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="19">
         <v>2.97798371315002</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="19">
         <v>2.67367768287658</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="19">
         <v>2.78690481185913</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="18">
         <v>3.22209668159484</v>
       </c>
       <c r="M5">
-        <f>AVERAGE(D5:L5)</f>
+        <f t="shared" si="0"/>
         <v>2.91953812705146</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="10">
         <v>2.7675</v>
       </c>
       <c r="O5">
-        <f>AVERAGE(F5,G5,H5,I5,J5,K5)</f>
+        <f t="shared" si="1"/>
         <v>2.76279882589976</v>
       </c>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="18">
         <v>3.24160766601562</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="18">
         <v>3.2353458404541</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="19">
         <v>2.7101879119873</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="19">
         <v>2.58928322792053</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="19">
         <v>2.82950592041015</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="19">
         <v>2.9840497970581</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="19">
         <v>2.67295050621032</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="19">
         <v>2.78196024894714</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="18">
         <v>3.22209668159484</v>
       </c>
       <c r="M6">
-        <f>AVERAGE(D6:L6)</f>
+        <f t="shared" si="0"/>
         <v>2.91855420006646</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="10">
         <v>2.765</v>
       </c>
       <c r="O6">
-        <f>AVERAGE(F6,G6,H6,I6,J6,K6)</f>
+        <f t="shared" si="1"/>
         <v>2.76132293542226</v>
       </c>
     </row>
     <row r="7" spans="2:15">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="18">
         <v>3.24160766601562</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="18">
         <v>3.2353458404541</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="19">
         <v>2.71503353118896</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="19">
         <v>2.58696699142456</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="19">
         <v>2.82127571105957</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="19">
         <v>2.98228979110717</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="19">
         <v>2.68308401107788</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="19">
         <v>2.78615927696228</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="18">
         <v>3.22209668159484</v>
       </c>
       <c r="M7">
-        <f>AVERAGE(D7:L7)</f>
+        <f t="shared" si="0"/>
         <v>2.91931772232055</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="10">
         <v>2.7575</v>
       </c>
       <c r="O7">
-        <f>AVERAGE(F7,G7,H7,I7,J7,K7)</f>
+        <f t="shared" si="1"/>
         <v>2.7624682188034</v>
       </c>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="18">
         <v>3.24160766601562</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="18">
         <v>3.2353458404541</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="19">
         <v>2.71525597572326</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="19">
         <v>2.59344410896301</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="19">
         <v>2.82168626785278</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="19">
         <v>2.95640182495117</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="19">
         <v>2.676283121109</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="19">
         <v>2.78643751144409</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="18">
         <v>3.22209668159484</v>
       </c>
       <c r="M8">
-        <f>AVERAGE(D8:L8)</f>
+        <f t="shared" si="0"/>
         <v>2.91650655534532</v>
       </c>
+      <c r="N8" s="10">
+        <v>2.71</v>
+      </c>
       <c r="O8">
-        <f>AVERAGE(F8,G8,H8,I8,J8,K8)</f>
+        <f t="shared" si="1"/>
         <v>2.75825146834055</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
+    <row r="9" spans="2:15">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="D9" s="18">
+        <v>3.24160766601562</v>
+      </c>
+      <c r="E9" s="18">
+        <v>3.2353458404541</v>
+      </c>
+      <c r="F9" s="19">
+        <v>2.67317247390747</v>
+      </c>
+      <c r="G9" s="19">
+        <v>2.56507635116577</v>
+      </c>
+      <c r="H9" s="19">
+        <v>2.79338526725769</v>
+      </c>
+      <c r="I9" s="19">
+        <v>2.95572543144226</v>
+      </c>
+      <c r="J9" s="19">
+        <v>2.63987255096435</v>
+      </c>
+      <c r="K9" s="19">
+        <v>2.7498025894165</v>
+      </c>
+      <c r="L9" s="18">
+        <v>3.22209668159484</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>2.89734276135762</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>2.72950577735901</v>
+      </c>
     </row>
     <row r="10" spans="2:12">
-      <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="L10" s="1"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="4:12">
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="L11" s="1"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="L11" s="16"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="22"/>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="9" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="9" t="s">
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="5" t="s">
+      <c r="L13" s="22"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="9" t="s">
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:12">
-      <c r="A14" s="5" t="s">
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="22"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="D15" s="22"/>
+      <c r="E15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="9" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K15" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:12">
-      <c r="A15" s="5" t="s">
+      <c r="L15" s="22"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D16" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E16" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L16" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="5" t="s">
+    <row r="17" spans="1:12">
+      <c r="A17" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C17" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9" t="s">
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="9" t="s">
+      <c r="G17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="9" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="8" t="s">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
-      <c r="A17" s="10" t="s">
+    <row r="18" spans="1:12">
+      <c r="A18" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9" t="s">
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="8" t="s">
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:12">
+      <c r="A19" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="9" t="s">
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H19" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I18" s="9" t="s">
+      <c r="I19" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="10" t="s">
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C20" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="9" t="s">
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="9" t="s">
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="5" t="s">
+      <c r="K20" s="10"/>
+      <c r="L20" s="22"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C21" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="9" t="s">
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" s="5" t="s">
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="22"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C22" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="9" t="s">
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I22" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="9" t="s">
+      <c r="J22" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" s="11" t="s">
+      <c r="K22" s="10"/>
+      <c r="L22" s="22"/>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B23" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="L22" s="1"/>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="12" t="s">
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="L23" s="16"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="12" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:1">
+      <c r="A27" s="25" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
-      <c r="A27" s="12" t="s">
+    <row r="28" spans="1:1">
+      <c r="A28" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
-      <c r="A28" s="12" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" s="25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="12" t="s">
+    <row r="30" spans="1:1">
+      <c r="A30" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
-      <c r="A30" s="12" t="s">
+    <row r="31" spans="1:1">
+      <c r="A31" s="25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="12" t="s">
+    <row r="32" spans="1:1">
+      <c r="A32" s="25" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
-      <c r="A32" s="12" t="s">
+    <row r="33" spans="1:1">
+      <c r="A33" s="25" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2247,14 +2356,314 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="4" width="10.7777777777778" customWidth="1"/>
+    <col min="5" max="5" width="16.4444444444444" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13" style="2" customWidth="1"/>
+    <col min="8" max="8" width="16.4444444444444" customWidth="1"/>
+    <col min="9" max="9" width="12.2222222222222" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3">
+        <v>5.21</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2.7825</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11">
+        <v>2.76613263289133</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H8" si="0">ABS(E3-B3)</f>
+        <v>0.0163673671086704</v>
+      </c>
+      <c r="I3" s="13">
+        <f t="shared" ref="I3:I8" si="1">H3/B3</f>
+        <v>0.00588225233016007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3">
+        <v>5.22</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2.775</v>
+      </c>
+      <c r="C4" s="10">
+        <f t="shared" ref="C4:C8" si="2">B4-B3</f>
+        <v>-0.00750000000000028</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" ref="D4:D8" si="3">C4/B3</f>
+        <v>-0.00269541778975751</v>
+      </c>
+      <c r="E4" s="11">
+        <v>2.76440143585205</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F9" si="4">E4-E3</f>
+        <v>-0.00173119703927993</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" ref="G4:G9" si="5">F4/E3</f>
+        <v>-0.000625854674752301</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.01059856414795</v>
+      </c>
+      <c r="I4" s="13">
+        <f t="shared" si="1"/>
+        <v>0.00381930239565766</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3">
+        <v>5.23</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2.7675</v>
+      </c>
+      <c r="C5" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.00749999999999984</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="3"/>
+        <v>-0.00270270270270265</v>
+      </c>
+      <c r="E5" s="11">
+        <v>2.76279882589976</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="4"/>
+        <v>-0.00160260995229011</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" si="5"/>
+        <v>-0.000579731268948698</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" si="0"/>
+        <v>0.00470117410024029</v>
+      </c>
+      <c r="I5" s="13">
+        <f t="shared" si="1"/>
+        <v>0.00169870789529911</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3">
+        <v>5.24</v>
+      </c>
+      <c r="B6" s="9">
+        <v>2.765</v>
+      </c>
+      <c r="C6" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.00249999999999995</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" si="3"/>
+        <v>-0.000903342366756983</v>
+      </c>
+      <c r="E6" s="11">
+        <v>2.76132293542226</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="4"/>
+        <v>-0.00147589047749985</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="5"/>
+        <v>-0.000534201210621696</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.0036770645777402</v>
+      </c>
+      <c r="I6" s="13">
+        <f t="shared" si="1"/>
+        <v>0.00132986060677765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3">
+        <v>5.25</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2.7575</v>
+      </c>
+      <c r="C7" s="10">
+        <f t="shared" si="2"/>
+        <v>-0.00750000000000028</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" si="3"/>
+        <v>-0.0027124773960218</v>
+      </c>
+      <c r="E7" s="11">
+        <v>2.7624682188034</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="4"/>
+        <v>0.00114528338114006</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="5"/>
+        <v>0.000414758942696764</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.00496821880340015</v>
+      </c>
+      <c r="I7" s="13">
+        <f t="shared" si="1"/>
+        <v>0.00180171126143251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3">
+        <v>5.26</v>
+      </c>
+      <c r="B8" s="15">
+        <v>2.71</v>
+      </c>
+      <c r="C8" s="10">
+        <f>B8-B7</f>
+        <v>-0.0474999999999999</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="3"/>
+        <v>-0.0172257479601087</v>
+      </c>
+      <c r="E8" s="11">
+        <v>2.75825146834055</v>
+      </c>
+      <c r="F8" s="9">
+        <f t="shared" si="4"/>
+        <v>-0.00421675046285008</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="5"/>
+        <v>-0.00152644306788681</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.0482514683405499</v>
+      </c>
+      <c r="I8" s="13">
+        <f t="shared" si="1"/>
+        <v>0.0178049698673616</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" spans="1:9">
+      <c r="A9" s="3">
+        <v>5.27</v>
+      </c>
+      <c r="B9" s="15">
+        <v>2.6974</v>
+      </c>
+      <c r="C9" s="10">
+        <f>B9-B8</f>
+        <v>-0.0125999999999999</v>
+      </c>
+      <c r="D9" s="13">
+        <f>C9/B8</f>
+        <v>-0.00464944649446492</v>
+      </c>
+      <c r="E9" s="11">
+        <v>2.72950577735901</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" si="4"/>
+        <v>-0.0287456909815433</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="5"/>
+        <v>-0.0104217078506035</v>
+      </c>
+      <c r="H9" s="9">
+        <f>ABS(E9-B9)</f>
+        <v>0.0321057773590101</v>
+      </c>
+      <c r="I9" s="13">
+        <f>H9/B9</f>
+        <v>0.0119024903088196</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>

</xml_diff>